<commit_message>
Atualização do documento de caso de teste para caso CT-c002 corrigido
</commit_message>
<xml_diff>
--- a/testes/cmproject_test_case - Diogenes - PS.xlsx
+++ b/testes/cmproject_test_case - Diogenes - PS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Github\cmproject\testes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJETOS SMARTGIT\cmproject\testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="851" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="851" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="216">
   <si>
     <t>Projeto de Teste</t>
   </si>
@@ -113,12 +113,6 @@
   </si>
   <si>
     <t>CT-a002</t>
-  </si>
-  <si>
-    <t>ALUGAR VEÍCULO COM PRAZO EM USO</t>
-  </si>
-  <si>
-    <t>QUE O SISTEMA RETORNE COM A MENSAGEM DE VEÍCULO INDISPONÍVEL PARA A DATA SELECIONADA</t>
   </si>
   <si>
     <t>CT-a003</t>
@@ -439,9 +433,6 @@
   </si>
   <si>
     <t>LISTA COM TODOS OS VEÍCULOS CADASTRADOS COM AS RESPECTIVAS IMAGENS</t>
-  </si>
-  <si>
-    <t>CAMPO IMAGEM NÃO RETORNA IMAGEM DO VEÍCULO</t>
   </si>
   <si>
     <t>Fazer login com campos "Email" ou "Senha" vazios</t>
@@ -587,9 +578,6 @@
 Data: DD/MM/YYYY</t>
   </si>
   <si>
-    <t>Não impede que veículo seja alugado estando em prazo de uso já utilizado.</t>
-  </si>
-  <si>
     <t>O VISITANTE SELECIONA VEICULO, CLICA EM ALUGAR .</t>
   </si>
   <si>
@@ -626,9 +614,6 @@
     <t>Tela deve exibir o comprovante de aluguél para ser impresso e poder retirar o veículo</t>
   </si>
   <si>
-    <t>Tela só exibe a mensagem de veículo alugado, mas comprovante não é disponibilizado</t>
-  </si>
-  <si>
     <t>CT-l001</t>
   </si>
   <si>
@@ -678,12 +663,30 @@
   </si>
   <si>
     <t>Pagina com o a localização da locadora exibida na tela</t>
+  </si>
+  <si>
+    <t>Comprovante de alugeul exibido com sucesso</t>
+  </si>
+  <si>
+    <t>ALUGAR VEÍCULO QUE ESTÁ LAUGADO</t>
+  </si>
+  <si>
+    <t>O VISITANTE ESCO NO BOTÃO  ALUGAR.</t>
+  </si>
+  <si>
+    <t>BOTÃO DE ALGAR DEVE ESTÁ DESABILITADO</t>
+  </si>
+  <si>
+    <t>Para um veiculo alugado o botão de alugar está desabilitado</t>
+  </si>
+  <si>
+    <t>MENSAGEM "email informado já cadastrado"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -762,7 +765,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -851,6 +854,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFDCE6F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -1065,7 +1074,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1263,6 +1272,9 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1287,7 +1299,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1406,7 +1418,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1444,7 +1456,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1516,7 +1528,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1793,11 +1805,11 @@
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="81" t="s">
+      <c r="E13" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
       <c r="H13" s="11"/>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
@@ -1806,9 +1818,9 @@
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
       <c r="H14" s="11"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
@@ -1828,11 +1840,11 @@
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="82" t="s">
+      <c r="E16" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="82"/>
-      <c r="G16" s="82"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="83"/>
       <c r="H16" s="11"/>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
@@ -1841,9 +1853,9 @@
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="82"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="83"/>
       <c r="H17" s="11"/>
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
@@ -1889,11 +1901,11 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="83" t="s">
+      <c r="E21" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
       <c r="H21" s="11"/>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
@@ -1902,11 +1914,11 @@
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="83" t="s">
+      <c r="E22" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="83"/>
-      <c r="G22" s="83"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
       <c r="H22" s="11"/>
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
@@ -1915,9 +1927,9 @@
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
       <c r="H23" s="11"/>
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
@@ -2089,8 +2101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2145,11 +2157,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2199,10 +2211,10 @@
         <v>25</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G6" s="80" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2214,27 +2226,27 @@
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
     </row>
-    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>28</v>
+        <v>211</v>
       </c>
       <c r="C8" s="45" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>24</v>
+        <v>212</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>29</v>
+        <v>213</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>183</v>
-      </c>
-      <c r="G8" s="48" t="s">
-        <v>184</v>
+        <v>180</v>
+      </c>
+      <c r="G8" s="80" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2248,25 +2260,25 @@
     </row>
     <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="45" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="45" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F10" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="G10" s="80" t="s">
         <v>183</v>
-      </c>
-      <c r="G10" s="80" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -2280,25 +2292,25 @@
     </row>
     <row r="12" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="45" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="45" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F12" s="47" t="s">
         <v>26</v>
       </c>
       <c r="G12" s="80" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -2312,25 +2324,25 @@
     </row>
     <row r="14" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="D14" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="E14" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="F14" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>41</v>
-      </c>
       <c r="G14" s="48" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -2344,25 +2356,25 @@
     </row>
     <row r="16" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="E16" s="46" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="C16" s="45" t="s">
-        <v>194</v>
-      </c>
-      <c r="D16" s="45" t="s">
-        <v>195</v>
-      </c>
-      <c r="E16" s="46" t="s">
-        <v>196</v>
-      </c>
       <c r="F16" s="47" t="s">
-        <v>183</v>
-      </c>
-      <c r="G16" s="48" t="s">
-        <v>197</v>
+        <v>180</v>
+      </c>
+      <c r="G16" s="80" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2466,7 +2478,7 @@
     </row>
     <row r="28" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" s="55"/>
       <c r="C28" s="55"/>
@@ -2486,7 +2498,7 @@
     </row>
     <row r="30" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B30" s="45"/>
       <c r="C30" s="45"/>
@@ -2506,7 +2518,7 @@
     </row>
     <row r="32" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B32" s="45"/>
       <c r="C32" s="55"/>
@@ -2526,7 +2538,7 @@
     </row>
     <row r="34" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="44" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B34" s="45"/>
       <c r="C34" s="45"/>
@@ -2546,7 +2558,7 @@
     </row>
     <row r="36" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36" s="45"/>
       <c r="C36" s="45"/>
@@ -2566,7 +2578,7 @@
     </row>
     <row r="38" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38" s="45"/>
       <c r="C38" s="45"/>
@@ -2586,7 +2598,7 @@
     </row>
     <row r="40" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B40" s="45"/>
       <c r="C40" s="45"/>
@@ -2606,7 +2618,7 @@
     </row>
     <row r="42" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B42" s="45"/>
       <c r="C42" s="45"/>
@@ -2626,7 +2638,7 @@
     </row>
     <row r="44" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="44" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B44" s="45"/>
       <c r="C44" s="45"/>
@@ -2646,7 +2658,7 @@
     </row>
     <row r="46" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="44" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B46" s="55"/>
       <c r="C46" s="55"/>
@@ -2660,7 +2672,7 @@
     </row>
     <row r="48" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B48" s="55"/>
       <c r="C48" s="55"/>
@@ -2674,7 +2686,7 @@
     </row>
     <row r="50" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B50" s="55"/>
       <c r="C50" s="55"/>
@@ -2688,7 +2700,7 @@
     </row>
     <row r="52" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B52" s="55"/>
       <c r="C52" s="55"/>
@@ -2702,7 +2714,7 @@
     </row>
     <row r="54" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54" s="45"/>
       <c r="C54" s="45"/>
@@ -2716,7 +2728,7 @@
     </row>
     <row r="56" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="44" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B56" s="45"/>
       <c r="C56" s="45"/>
@@ -2730,7 +2742,7 @@
     </row>
     <row r="58" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B58" s="45"/>
       <c r="C58" s="45"/>
@@ -2744,7 +2756,7 @@
     </row>
     <row r="60" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B60" s="45"/>
       <c r="C60" s="45"/>
@@ -2755,7 +2767,7 @@
     </row>
     <row r="62" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B62" s="45"/>
       <c r="C62" s="45"/>
@@ -2769,7 +2781,7 @@
     </row>
     <row r="64" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B64" s="45"/>
       <c r="C64" s="45"/>
@@ -2783,7 +2795,7 @@
     </row>
     <row r="66" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B66" s="45"/>
       <c r="C66" s="45"/>
@@ -2913,7 +2925,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="31"/>
@@ -2927,11 +2939,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
+      <c r="B3" s="86" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2966,25 +2978,25 @@
     </row>
     <row r="6" spans="1:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="D6" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="E6" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="F6" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="G6" s="75" t="s">
         <v>68</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="75" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2998,25 +3010,25 @@
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" s="44" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="G8" s="75" t="s">
         <v>74</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="75" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3030,25 +3042,25 @@
     </row>
     <row r="10" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B10" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="C10" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="E10" s="72" t="s">
-        <v>140</v>
-      </c>
       <c r="F10" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G10" s="74" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3296,8 +3308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3338,7 +3350,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="31"/>
@@ -3352,11 +3364,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
+      <c r="B3" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3391,25 +3403,25 @@
     </row>
     <row r="6" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="71" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6" s="45" t="s">
+      <c r="E6" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="G6" s="64" t="s">
         <v>83</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="64" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -3423,25 +3435,25 @@
     </row>
     <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="D8" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="E8" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>90</v>
-      </c>
       <c r="F8" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="48" t="s">
-        <v>91</v>
+        <v>82</v>
+      </c>
+      <c r="G8" s="90" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3455,25 +3467,25 @@
     </row>
     <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="D10" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>95</v>
-      </c>
       <c r="E10" s="46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G10" s="64" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3487,25 +3499,25 @@
     </row>
     <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="E12" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="45" t="s">
+      <c r="F12" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" s="47" t="s">
-        <v>100</v>
-      </c>
       <c r="G12" s="64" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3519,25 +3531,25 @@
     </row>
     <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="71" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B14" s="71" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C14" s="71" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D14" s="71" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F14" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G14" s="74" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -3551,25 +3563,25 @@
     </row>
     <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="71" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B16" s="71" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C16" s="71" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D16" s="71" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G16" s="74" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -3583,25 +3595,25 @@
     </row>
     <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="71" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B18" s="71" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C18" s="71" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D18" s="71" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E18" s="72" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F18" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G18" s="74" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -3615,25 +3627,25 @@
     </row>
     <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="71" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B20" s="71" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C20" s="71" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D20" s="71" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E20" s="72" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F20" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G20" s="74" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -3647,25 +3659,25 @@
     </row>
     <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="71" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B22" s="71" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C22" s="71" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D22" s="71" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E22" s="72" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F22" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G22" s="74" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -3679,25 +3691,25 @@
     </row>
     <row r="24" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A24" s="71" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B24" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="E24" s="72" t="s">
+        <v>156</v>
+      </c>
+      <c r="F24" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="C24" s="71" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="71" t="s">
-        <v>158</v>
-      </c>
-      <c r="E24" s="72" t="s">
-        <v>159</v>
-      </c>
-      <c r="F24" s="73" t="s">
-        <v>160</v>
-      </c>
       <c r="G24" s="74" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3755,7 +3767,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="31"/>
@@ -3769,11 +3781,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
+      <c r="B3" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3808,25 +3820,25 @@
     </row>
     <row r="6" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="45" t="s">
+      <c r="D6" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="F6" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="G6" s="64" t="s">
         <v>83</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="64" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -3840,25 +3852,25 @@
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B8" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="45" t="s">
-        <v>106</v>
-      </c>
       <c r="E8" s="46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G8" s="48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3872,25 +3884,25 @@
     </row>
     <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>109</v>
-      </c>
       <c r="E10" s="46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G10" s="64" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3904,25 +3916,25 @@
     </row>
     <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D12" s="45" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F12" s="47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G12" s="64" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3936,25 +3948,25 @@
     </row>
     <row r="14" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A14" s="76" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B14" s="76" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C14" s="76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D14" s="76" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F14" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G14" s="74" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -3968,25 +3980,25 @@
     </row>
     <row r="16" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A16" s="76" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B16" s="76" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C16" s="76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D16" s="76" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G16" s="74" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -4000,25 +4012,25 @@
     </row>
     <row r="18" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A18" s="76" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B18" s="76" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C18" s="76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D18" s="76" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E18" s="72" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F18" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G18" s="74" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -4032,25 +4044,25 @@
     </row>
     <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="76" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B20" s="76" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C20" s="76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D20" s="76" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E20" s="72" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F20" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G20" s="74" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -4064,25 +4076,25 @@
     </row>
     <row r="22" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A22" s="76" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B22" s="76" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C22" s="76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D22" s="76" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E22" s="72" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F22" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G22" s="74" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -4096,25 +4108,25 @@
     </row>
     <row r="24" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A24" s="76" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B24" s="76" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C24" s="76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D24" s="76" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E24" s="72" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G24" s="74" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -4128,25 +4140,25 @@
     </row>
     <row r="26" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A26" s="76" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B26" s="76" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C26" s="76" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D26" s="76" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E26" s="72" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F26" s="73" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G26" s="74" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -4162,8 +4174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4204,7 +4216,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="31"/>
@@ -4218,11 +4230,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="88" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
+      <c r="B3" s="89" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -4257,25 +4269,25 @@
     </row>
     <row r="6" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="D6" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="E6" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>117</v>
-      </c>
       <c r="G6" s="64" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4289,25 +4301,25 @@
     </row>
     <row r="8" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="E8" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="F8" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>117</v>
-      </c>
       <c r="G8" s="64" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -4321,25 +4333,25 @@
     </row>
     <row r="10" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="F10" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10" s="46" t="s">
+      <c r="G10" s="48" t="s">
         <v>124</v>
-      </c>
-      <c r="F10" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="48" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -4353,25 +4365,25 @@
     </row>
     <row r="12" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="D12" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="E12" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="F12" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="E12" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="F12" s="47" t="s">
-        <v>132</v>
-      </c>
       <c r="G12" s="64" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -4385,25 +4397,25 @@
     </row>
     <row r="14" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="B14" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" s="45" t="s">
+      <c r="F14" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="64" t="s">
         <v>129</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="E14" s="46" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>132</v>
-      </c>
-      <c r="G14" s="48" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -4417,25 +4429,25 @@
     </row>
     <row r="16" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A16" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="F16" s="52" t="s">
         <v>203</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="G16" s="81" t="s">
         <v>204</v>
-      </c>
-      <c r="C16" s="45" t="s">
-        <v>205</v>
-      </c>
-      <c r="D16" s="45" t="s">
-        <v>206</v>
-      </c>
-      <c r="E16" s="46" t="s">
-        <v>207</v>
-      </c>
-      <c r="F16" s="52" t="s">
-        <v>208</v>
-      </c>
-      <c r="G16" s="89" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -4781,7 +4793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -4822,7 +4834,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="31"/>
@@ -4836,11 +4848,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="85" t="s">
-        <v>191</v>
-      </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
+      <c r="B3" s="86" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -4875,25 +4887,25 @@
     </row>
     <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="78" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B6" s="79" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C6" s="79" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="79" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F6" s="47" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4907,25 +4919,25 @@
     </row>
     <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A8" s="78" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B8" s="79" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C8" s="78" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D8" s="79" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F8" s="47" t="s">
         <v>26</v>
       </c>
       <c r="G8" s="75" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Atualização do documento de caso de teste para caso CT-a005 corrigido
</commit_message>
<xml_diff>
--- a/testes/cmproject_test_case - Diogenes - PS.xlsx
+++ b/testes/cmproject_test_case - Diogenes - PS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="851" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="851" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -590,9 +590,6 @@
     <t>Ao clicar para alugar sem estar com sessão iniciada, será redirecionado para a tela de login</t>
   </si>
   <si>
-    <t>Permitindo que qualquer prazo seja inserido para o aluguel</t>
-  </si>
-  <si>
     <t>Encontre-nos</t>
   </si>
   <si>
@@ -681,6 +678,9 @@
   </si>
   <si>
     <t>MENSAGEM "email informado já cadastrado"</t>
+  </si>
+  <si>
+    <t>Mensagem: O campo 'Data de retirada' deve ter uma data maior que atual</t>
   </si>
 </sst>
 </file>
@@ -1275,6 +1275,9 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1298,9 +1301,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1805,11 +1805,11 @@
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="82" t="s">
+      <c r="E13" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
       <c r="H13" s="11"/>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
@@ -1818,9 +1818,9 @@
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
       <c r="H14" s="11"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
@@ -1840,11 +1840,11 @@
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="83" t="s">
+      <c r="E16" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="84"/>
       <c r="H16" s="11"/>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
@@ -1853,9 +1853,9 @@
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
-      <c r="G17" s="83"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84"/>
       <c r="H17" s="11"/>
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
@@ -1901,11 +1901,11 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="84" t="s">
+      <c r="E21" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="84"/>
-      <c r="G21" s="84"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
       <c r="H21" s="11"/>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
@@ -1914,11 +1914,11 @@
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="84" t="s">
+      <c r="E22" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="85"/>
       <c r="H22" s="11"/>
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
@@ -1927,9 +1927,9 @@
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="85"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="85"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
       <c r="H23" s="11"/>
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
@@ -2101,8 +2101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2157,11 +2157,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2231,22 +2231,22 @@
         <v>27</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C8" s="45" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="E8" s="46" t="s">
         <v>212</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>213</v>
       </c>
       <c r="F8" s="47" t="s">
         <v>180</v>
       </c>
       <c r="G8" s="80" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2341,8 +2341,8 @@
       <c r="F14" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="48" t="s">
-        <v>185</v>
+      <c r="G14" s="80" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -2356,25 +2356,25 @@
     </row>
     <row r="16" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="C16" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="D16" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="E16" s="46" t="s">
         <v>191</v>
-      </c>
-      <c r="E16" s="46" t="s">
-        <v>192</v>
       </c>
       <c r="F16" s="47" t="s">
         <v>180</v>
       </c>
       <c r="G16" s="80" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2875,7 +2875,7 @@
     <hyperlink ref="F16" r:id="rId4" display="LOGIN: cimara@gmail.com_x000a_SENHA: 1234"/>
   </hyperlinks>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2939,11 +2939,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -3308,7 +3308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3364,11 +3364,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3452,8 +3452,8 @@
       <c r="F8" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="90" t="s">
-        <v>215</v>
+      <c r="G8" s="82" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3726,7 +3726,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3781,11 +3781,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -3869,8 +3869,8 @@
       <c r="F8" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="48" t="s">
-        <v>89</v>
+      <c r="G8" s="82" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -4174,8 +4174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4230,11 +4230,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="66"/>
@@ -4429,25 +4429,25 @@
     </row>
     <row r="16" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A16" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="C16" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="D16" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="E16" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="F16" s="52" t="s">
         <v>202</v>
       </c>
-      <c r="F16" s="52" t="s">
+      <c r="G16" s="81" t="s">
         <v>203</v>
-      </c>
-      <c r="G16" s="81" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -4834,7 +4834,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="31"/>
@@ -4848,11 +4848,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="86" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
+      <c r="B3" s="87" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -4887,25 +4887,25 @@
     </row>
     <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="78" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="79" t="s">
         <v>193</v>
-      </c>
-      <c r="B6" s="79" t="s">
-        <v>194</v>
       </c>
       <c r="C6" s="79" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="79" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="46" t="s">
         <v>195</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>196</v>
       </c>
       <c r="F6" s="47" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4919,25 +4919,25 @@
     </row>
     <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A8" s="78" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="79" t="s">
         <v>205</v>
       </c>
-      <c r="B8" s="79" t="s">
+      <c r="C8" s="78" t="s">
         <v>206</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="D8" s="79" t="s">
         <v>207</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="E8" s="46" t="s">
         <v>208</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>209</v>
       </c>
       <c r="F8" s="47" t="s">
         <v>26</v>
       </c>
       <c r="G8" s="75" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Atualização do documento de caso de teste para caso CT-a003 corrigido
</commit_message>
<xml_diff>
--- a/testes/cmproject_test_case - Diogenes - PS.xlsx
+++ b/testes/cmproject_test_case - Diogenes - PS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="851" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="851"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -405,9 +405,6 @@
     <t>ARQUIVO DE IMAGEM NO CAMPO DO FORMULÁRIO</t>
   </si>
   <si>
-    <t>IMAGEM NÃO SALVA E NEM SENDO EXIBIDA NA LISTA DE NOSSOS VEÍCULOS.</t>
-  </si>
-  <si>
     <t>CT-d001</t>
   </si>
   <si>
@@ -681,6 +678,9 @@
   </si>
   <si>
     <t>Mensagem: O campo 'Data de retirada' deve ter uma data maior que atual</t>
+  </si>
+  <si>
+    <t>IMAGEM É SALVA E ESTÁ SENDO EXIBIDA NA LISTA DE NOSSOS VEÍCULOS.</t>
   </si>
 </sst>
 </file>
@@ -765,7 +765,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -824,12 +824,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF1F497D"/>
         <bgColor rgb="FF003366"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
@@ -1074,7 +1068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1177,9 +1171,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1225,7 +1216,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1251,31 +1242,31 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1680,7 +1671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E23" activeCellId="1" sqref="A6:XFD6 E23:G23"/>
     </sheetView>
   </sheetViews>
@@ -1805,11 +1796,11 @@
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="83" t="s">
+      <c r="E13" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
       <c r="H13" s="11"/>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
@@ -1818,9 +1809,9 @@
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
       <c r="H14" s="11"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
@@ -1840,11 +1831,11 @@
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="84" t="s">
+      <c r="E16" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="83"/>
       <c r="H16" s="11"/>
       <c r="I16" s="5"/>
       <c r="J16" s="6"/>
@@ -1853,9 +1844,9 @@
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="10"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="83"/>
       <c r="H17" s="11"/>
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
@@ -1901,11 +1892,11 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="85" t="s">
+      <c r="E21" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="85"/>
-      <c r="G21" s="85"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
       <c r="H21" s="11"/>
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
@@ -1914,11 +1905,11 @@
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="85" t="s">
+      <c r="E22" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="85"/>
-      <c r="G22" s="85"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
       <c r="H22" s="11"/>
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
@@ -1927,9 +1918,9 @@
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="10"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
       <c r="H23" s="11"/>
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
@@ -2101,9 +2092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2157,11 +2146,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2211,52 +2200,52 @@
         <v>25</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="G6" s="80" t="s">
         <v>179</v>
       </c>
+      <c r="G6" s="79" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
     </row>
     <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C8" s="45" t="s">
         <v>23</v>
       </c>
       <c r="D8" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="F8" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="G8" s="79" t="s">
         <v>212</v>
       </c>
-      <c r="F8" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="G8" s="80" t="s">
-        <v>213</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
     </row>
     <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
@@ -2269,26 +2258,26 @@
         <v>23</v>
       </c>
       <c r="D10" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="E10" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="F10" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" s="79" t="s">
         <v>182</v>
       </c>
-      <c r="F10" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="G10" s="80" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="49"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
     </row>
     <row r="12" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
@@ -2309,18 +2298,18 @@
       <c r="F12" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="80" t="s">
-        <v>184</v>
+      <c r="G12" s="79" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="44" t="s">
@@ -2341,50 +2330,50 @@
       <c r="F14" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="80" t="s">
-        <v>215</v>
+      <c r="G14" s="79" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
+      <c r="A15" s="48"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
     </row>
     <row r="16" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="C16" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="D16" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="E16" s="46" t="s">
         <v>190</v>
       </c>
-      <c r="E16" s="46" t="s">
-        <v>191</v>
-      </c>
       <c r="F16" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="G16" s="80" t="s">
-        <v>209</v>
+        <v>179</v>
+      </c>
+      <c r="G16" s="79" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="49"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
     </row>
     <row r="18" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="44"/>
@@ -2392,109 +2381,109 @@
       <c r="C18" s="45"/>
       <c r="D18" s="45"/>
       <c r="E18" s="46"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="53"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="54"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
     </row>
     <row r="20" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="44"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="57"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="59"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
     </row>
     <row r="22" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="44"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="58"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="57"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="61"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
     </row>
     <row r="24" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="44"/>
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="58"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="57"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="61"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
     </row>
     <row r="26" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="44"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="58"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="57"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="54"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
+      <c r="A27" s="53"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
     </row>
     <row r="28" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="58"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="57"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="54"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
     </row>
     <row r="30" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44" t="s">
@@ -2502,39 +2491,39 @@
       </c>
       <c r="B30" s="45"/>
       <c r="C30" s="45"/>
-      <c r="D30" s="55"/>
+      <c r="D30" s="54"/>
       <c r="E30" s="46"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="53"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="52"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="49"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
     </row>
     <row r="32" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="44" t="s">
         <v>42</v>
       </c>
       <c r="B32" s="45"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="53"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="52"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="49"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
     </row>
     <row r="34" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="44" t="s">
@@ -2542,19 +2531,19 @@
       </c>
       <c r="B34" s="45"/>
       <c r="C34" s="45"/>
-      <c r="D34" s="55"/>
+      <c r="D34" s="54"/>
       <c r="E34" s="46"/>
       <c r="F34" s="47"/>
-      <c r="G34" s="53"/>
+      <c r="G34" s="52"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="49"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
     </row>
     <row r="36" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44" t="s">
@@ -2562,19 +2551,19 @@
       </c>
       <c r="B36" s="45"/>
       <c r="C36" s="45"/>
-      <c r="D36" s="55"/>
+      <c r="D36" s="54"/>
       <c r="E36" s="46"/>
       <c r="F36" s="47"/>
-      <c r="G36" s="53"/>
+      <c r="G36" s="52"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="49"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="50"/>
+      <c r="A37" s="48"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
     </row>
     <row r="38" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="44" t="s">
@@ -2582,19 +2571,19 @@
       </c>
       <c r="B38" s="45"/>
       <c r="C38" s="45"/>
-      <c r="D38" s="55"/>
+      <c r="D38" s="54"/>
       <c r="E38" s="46"/>
       <c r="F38" s="47"/>
-      <c r="G38" s="53"/>
+      <c r="G38" s="52"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="49"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
     </row>
     <row r="40" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="44" t="s">
@@ -2602,19 +2591,19 @@
       </c>
       <c r="B40" s="45"/>
       <c r="C40" s="45"/>
-      <c r="D40" s="55"/>
+      <c r="D40" s="54"/>
       <c r="E40" s="46"/>
       <c r="F40" s="47"/>
-      <c r="G40" s="53"/>
+      <c r="G40" s="52"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="49"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
+      <c r="A41" s="48"/>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
     </row>
     <row r="42" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="44" t="s">
@@ -2622,13 +2611,13 @@
       </c>
       <c r="B42" s="45"/>
       <c r="C42" s="45"/>
-      <c r="D42" s="55"/>
+      <c r="D42" s="54"/>
       <c r="E42" s="46"/>
       <c r="F42" s="47"/>
-      <c r="G42" s="53"/>
+      <c r="G42" s="52"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="62"/>
+      <c r="A43" s="61"/>
       <c r="B43" s="28"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
@@ -2642,13 +2631,13 @@
       </c>
       <c r="B44" s="45"/>
       <c r="C44" s="45"/>
-      <c r="D44" s="55"/>
+      <c r="D44" s="54"/>
       <c r="E44" s="46"/>
       <c r="F44" s="47"/>
-      <c r="G44" s="53"/>
+      <c r="G44" s="52"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="62"/>
+      <c r="A45" s="61"/>
       <c r="B45" s="28"/>
       <c r="C45" s="28"/>
       <c r="D45" s="28"/>
@@ -2660,57 +2649,57 @@
       <c r="A46" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="58"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="57"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="62"/>
+      <c r="A47" s="61"/>
     </row>
     <row r="48" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="58"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="57"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="62"/>
+      <c r="A49" s="61"/>
     </row>
     <row r="50" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="58"/>
+      <c r="B50" s="54"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="57"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="62"/>
+      <c r="A51" s="61"/>
     </row>
     <row r="52" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="55"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="58"/>
+      <c r="B52" s="54"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="57"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="62"/>
+      <c r="A53" s="61"/>
     </row>
     <row r="54" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="44" t="s">
@@ -2721,10 +2710,10 @@
       <c r="D54" s="45"/>
       <c r="E54" s="46"/>
       <c r="F54" s="47"/>
-      <c r="G54" s="53"/>
+      <c r="G54" s="52"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="62"/>
+      <c r="A55" s="61"/>
     </row>
     <row r="56" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="44" t="s">
@@ -2735,10 +2724,10 @@
       <c r="D56" s="45"/>
       <c r="E56" s="46"/>
       <c r="F56" s="47"/>
-      <c r="G56" s="53"/>
+      <c r="G56" s="52"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="62"/>
+      <c r="A57" s="61"/>
     </row>
     <row r="58" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="44" t="s">
@@ -2749,10 +2738,10 @@
       <c r="D58" s="45"/>
       <c r="E58" s="46"/>
       <c r="F58" s="47"/>
-      <c r="G58" s="53"/>
+      <c r="G58" s="52"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="62"/>
+      <c r="A59" s="61"/>
     </row>
     <row r="60" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="44" t="s">
@@ -2760,10 +2749,10 @@
       </c>
       <c r="B60" s="45"/>
       <c r="C60" s="45"/>
-      <c r="D60" s="63"/>
+      <c r="D60" s="62"/>
       <c r="E60" s="46"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="58"/>
+      <c r="F60" s="56"/>
+      <c r="G60" s="57"/>
     </row>
     <row r="62" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="44" t="s">
@@ -2773,11 +2762,11 @@
       <c r="C62" s="45"/>
       <c r="D62" s="45"/>
       <c r="E62" s="46"/>
-      <c r="F62" s="57"/>
-      <c r="G62" s="58"/>
+      <c r="F62" s="56"/>
+      <c r="G62" s="57"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="49"/>
+      <c r="A63" s="48"/>
     </row>
     <row r="64" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="44" t="s">
@@ -2787,11 +2776,11 @@
       <c r="C64" s="45"/>
       <c r="D64" s="45"/>
       <c r="E64" s="46"/>
-      <c r="F64" s="57"/>
-      <c r="G64" s="58"/>
+      <c r="F64" s="56"/>
+      <c r="G64" s="57"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="49"/>
+      <c r="A65" s="48"/>
     </row>
     <row r="66" spans="1:7" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="44" t="s">
@@ -2801,68 +2790,68 @@
       <c r="C66" s="45"/>
       <c r="D66" s="45"/>
       <c r="E66" s="46"/>
-      <c r="F66" s="57"/>
-      <c r="G66" s="58"/>
+      <c r="F66" s="56"/>
+      <c r="G66" s="57"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="49"/>
+      <c r="A67" s="48"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="44"/>
-      <c r="B68" s="55"/>
-      <c r="C68" s="55"/>
-      <c r="D68" s="55"/>
-      <c r="E68" s="56"/>
-      <c r="F68" s="57"/>
-      <c r="G68" s="58"/>
+      <c r="B68" s="54"/>
+      <c r="C68" s="54"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="56"/>
+      <c r="G68" s="57"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="49"/>
+      <c r="A69" s="48"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="44"/>
-      <c r="B70" s="55"/>
-      <c r="C70" s="55"/>
-      <c r="D70" s="55"/>
-      <c r="E70" s="56"/>
-      <c r="F70" s="57"/>
-      <c r="G70" s="58"/>
+      <c r="B70" s="54"/>
+      <c r="C70" s="54"/>
+      <c r="D70" s="54"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="56"/>
+      <c r="G70" s="57"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="49"/>
+      <c r="A71" s="48"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="44"/>
-      <c r="B72" s="55"/>
-      <c r="C72" s="55"/>
-      <c r="D72" s="55"/>
-      <c r="E72" s="56"/>
-      <c r="F72" s="57"/>
-      <c r="G72" s="58"/>
+      <c r="B72" s="54"/>
+      <c r="C72" s="54"/>
+      <c r="D72" s="54"/>
+      <c r="E72" s="55"/>
+      <c r="F72" s="56"/>
+      <c r="G72" s="57"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="49"/>
+      <c r="A73" s="48"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="44"/>
-      <c r="B74" s="55"/>
-      <c r="C74" s="55"/>
-      <c r="D74" s="55"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="57"/>
-      <c r="G74" s="58"/>
+      <c r="B74" s="54"/>
+      <c r="C74" s="54"/>
+      <c r="D74" s="54"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="56"/>
+      <c r="G74" s="57"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="49"/>
+      <c r="A75" s="48"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="44"/>
-      <c r="B76" s="55"/>
-      <c r="C76" s="55"/>
-      <c r="D76" s="55"/>
-      <c r="E76" s="56"/>
-      <c r="F76" s="57"/>
-      <c r="G76" s="58"/>
+      <c r="B76" s="54"/>
+      <c r="C76" s="54"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="55"/>
+      <c r="F76" s="56"/>
+      <c r="G76" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2939,11 +2928,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -2995,18 +2984,18 @@
       <c r="F6" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="75" t="s">
+      <c r="G6" s="74" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
@@ -3027,269 +3016,269 @@
       <c r="F8" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="G8" s="75" t="s">
+      <c r="G8" s="74" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="54"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
     </row>
     <row r="10" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B10" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="D10" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="E10" s="71" t="s">
         <v>136</v>
       </c>
-      <c r="E10" s="72" t="s">
-        <v>137</v>
-      </c>
-      <c r="F10" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G10" s="74" t="s">
-        <v>137</v>
+      <c r="F10" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G10" s="73" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="59"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
     </row>
     <row r="12" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="58"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="57"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="61"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="44"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="58"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="61"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
     </row>
     <row r="16" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="44"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="58"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="57"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="54"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
     </row>
     <row r="18" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="44"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="58"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="57"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="54"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
     </row>
     <row r="20" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="44"/>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
-      <c r="D20" s="55"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="46"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="53"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
     </row>
     <row r="22" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="44"/>
       <c r="B22" s="45"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="53"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="52"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
     </row>
     <row r="24" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="44"/>
       <c r="B24" s="45"/>
       <c r="C24" s="45"/>
-      <c r="D24" s="55"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="46"/>
       <c r="F24" s="47"/>
-      <c r="G24" s="53"/>
+      <c r="G24" s="52"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="49"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
     </row>
     <row r="26" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="44"/>
       <c r="B26" s="45"/>
       <c r="C26" s="45"/>
-      <c r="D26" s="55"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="46"/>
       <c r="F26" s="47"/>
-      <c r="G26" s="53"/>
+      <c r="G26" s="52"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
     </row>
     <row r="28" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
-      <c r="D28" s="55"/>
+      <c r="D28" s="54"/>
       <c r="E28" s="46"/>
       <c r="F28" s="47"/>
-      <c r="G28" s="53"/>
+      <c r="G28" s="52"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="44"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="58"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="57"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="49"/>
+      <c r="A31" s="48"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="44"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="58"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="57"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="49"/>
+      <c r="A33" s="48"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="44"/>
-      <c r="B34" s="55"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="58"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="57"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="49"/>
+      <c r="A35" s="48"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="44"/>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="58"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="57"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="49"/>
+      <c r="A37" s="48"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="44"/>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="58"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3320,7 +3309,7 @@
     <col min="4" max="4" width="28.42578125"/>
     <col min="5" max="5" width="33.42578125"/>
     <col min="6" max="6" width="25.85546875"/>
-    <col min="7" max="7" width="26.7109375" style="65"/>
+    <col min="7" max="7" width="26.7109375" style="64"/>
     <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
@@ -3358,25 +3347,25 @@
         <v>12</v>
       </c>
       <c r="F2" s="32"/>
-      <c r="G2" s="66"/>
+      <c r="G2" s="65"/>
     </row>
     <row r="3" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
-      <c r="G3" s="66"/>
+      <c r="G3" s="65"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E4" s="36"/>
       <c r="F4" s="37"/>
-      <c r="G4" s="67"/>
+      <c r="G4" s="66"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
@@ -3408,8 +3397,8 @@
       <c r="B6" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="71" t="s">
-        <v>135</v>
+      <c r="C6" s="70" t="s">
+        <v>134</v>
       </c>
       <c r="D6" s="45" t="s">
         <v>80</v>
@@ -3420,18 +3409,18 @@
       <c r="F6" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="63" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="67"/>
     </row>
     <row r="8" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
@@ -3452,18 +3441,18 @@
       <c r="F8" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="82" t="s">
-        <v>214</v>
+      <c r="G8" s="81" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="68"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="67"/>
     </row>
     <row r="10" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
@@ -3484,18 +3473,18 @@
       <c r="F10" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="64" t="s">
+      <c r="G10" s="63" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="49"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="68"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
@@ -3516,200 +3505,200 @@
       <c r="F12" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="G12" s="64" t="s">
+      <c r="G12" s="63" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="68"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="71" t="s">
+      <c r="A14" s="70" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="70" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14" s="73" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="48"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="67"/>
+    </row>
+    <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="70" t="s">
         <v>158</v>
       </c>
-      <c r="B14" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="E14" s="72" t="s">
+      <c r="B16" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="F14" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G14" s="74" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="68"/>
-    </row>
-    <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="71" t="s">
+      <c r="C16" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="F16" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" s="73" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="53"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="67"/>
+    </row>
+    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="70" t="s">
         <v>159</v>
       </c>
-      <c r="B16" s="71" t="s">
-        <v>142</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="D16" s="71" t="s">
-        <v>143</v>
-      </c>
-      <c r="E16" s="72" t="s">
+      <c r="B18" s="70" t="s">
         <v>144</v>
       </c>
-      <c r="F16" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G16" s="74" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="54"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="68"/>
-    </row>
-    <row r="18" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="71" t="s">
+      <c r="C18" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="70" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="71" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G18" s="73" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="58"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="67"/>
+    </row>
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="B18" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="D18" s="71" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" s="72" t="s">
+      <c r="B20" s="70" t="s">
         <v>147</v>
       </c>
-      <c r="F18" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" s="74" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="59"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="68"/>
-    </row>
-    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="71" t="s">
+      <c r="C20" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="70" t="s">
+        <v>148</v>
+      </c>
+      <c r="E20" s="71" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="73" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="60"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="67"/>
+    </row>
+    <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="B20" s="71" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" s="71" t="s">
-        <v>149</v>
-      </c>
-      <c r="E20" s="72" t="s">
+      <c r="B22" s="70" t="s">
         <v>150</v>
       </c>
-      <c r="F20" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G20" s="74" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="61"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="68"/>
-    </row>
-    <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="71" t="s">
+      <c r="C22" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" s="73" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="60"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="67"/>
+    </row>
+    <row r="24" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="B22" s="71" t="s">
-        <v>151</v>
-      </c>
-      <c r="C22" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="D22" s="71" t="s">
-        <v>152</v>
-      </c>
-      <c r="E22" s="72" t="s">
+      <c r="B24" s="70" t="s">
         <v>153</v>
       </c>
-      <c r="F22" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G22" s="74" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="61"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="68"/>
-    </row>
-    <row r="24" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="71" t="s">
-        <v>163</v>
-      </c>
-      <c r="B24" s="71" t="s">
+      <c r="C24" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="70" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="D24" s="71" t="s">
+      <c r="E24" s="71" t="s">
         <v>155</v>
       </c>
-      <c r="E24" s="72" t="s">
+      <c r="F24" s="72" t="s">
         <v>156</v>
       </c>
-      <c r="F24" s="73" t="s">
-        <v>157</v>
-      </c>
-      <c r="G24" s="74" t="s">
-        <v>156</v>
+      <c r="G24" s="73" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3737,7 +3726,7 @@
     <col min="4" max="4" width="28.42578125"/>
     <col min="5" max="5" width="33.42578125"/>
     <col min="6" max="6" width="25.85546875"/>
-    <col min="7" max="7" width="26.7109375" style="65"/>
+    <col min="7" max="7" width="26.7109375" style="64"/>
     <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
@@ -3775,25 +3764,25 @@
         <v>12</v>
       </c>
       <c r="F2" s="32"/>
-      <c r="G2" s="66"/>
+      <c r="G2" s="65"/>
     </row>
     <row r="3" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="88" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
-      <c r="G3" s="66"/>
+      <c r="G3" s="65"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E4" s="36"/>
       <c r="F4" s="37"/>
-      <c r="G4" s="67"/>
+      <c r="G4" s="66"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
@@ -3837,18 +3826,18 @@
       <c r="F6" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="63" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="67"/>
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
@@ -3869,18 +3858,18 @@
       <c r="F8" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="82" t="s">
-        <v>214</v>
+      <c r="G8" s="81" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="68"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="67"/>
     </row>
     <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
@@ -3901,18 +3890,18 @@
       <c r="F10" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="64" t="s">
+      <c r="G10" s="63" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="49"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="68"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
@@ -3933,232 +3922,232 @@
       <c r="F12" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="G12" s="64" t="s">
+      <c r="G12" s="63" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="68"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="75" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="75" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" s="71" t="s">
+        <v>165</v>
+      </c>
+      <c r="F14" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14" s="73" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="48"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="76"/>
+    </row>
+    <row r="16" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="B14" s="76" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="D14" s="76" t="s">
-        <v>165</v>
-      </c>
-      <c r="E14" s="72" t="s">
+      <c r="B16" s="75" t="s">
         <v>166</v>
       </c>
-      <c r="F14" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G14" s="74" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="77"/>
-    </row>
-    <row r="16" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="76" t="s">
+      <c r="C16" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="75" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" s="73" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="48"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="67"/>
+    </row>
+    <row r="18" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="75" t="s">
         <v>159</v>
       </c>
-      <c r="B16" s="76" t="s">
-        <v>167</v>
-      </c>
-      <c r="C16" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="D16" s="76" t="s">
+      <c r="B18" s="75" t="s">
         <v>168</v>
       </c>
-      <c r="E16" s="72" t="s">
-        <v>141</v>
-      </c>
-      <c r="F16" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G16" s="74" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="49"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="68"/>
-    </row>
-    <row r="18" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="76" t="s">
+      <c r="C18" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="E18" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="F18" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G18" s="73" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="53"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="67"/>
+    </row>
+    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="75" t="s">
         <v>160</v>
       </c>
-      <c r="B18" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="C18" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="D18" s="76" t="s">
+      <c r="B20" s="75" t="s">
         <v>170</v>
       </c>
-      <c r="E18" s="72" t="s">
-        <v>144</v>
-      </c>
-      <c r="F18" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" s="74" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="54"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="68"/>
-    </row>
-    <row r="20" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="76" t="s">
+      <c r="C20" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="75" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="71" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="73" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="58"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="67"/>
+    </row>
+    <row r="22" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="B20" s="76" t="s">
+      <c r="B22" s="75" t="s">
         <v>171</v>
       </c>
-      <c r="C20" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" s="76" t="s">
-        <v>146</v>
-      </c>
-      <c r="E20" s="72" t="s">
-        <v>147</v>
-      </c>
-      <c r="F20" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G20" s="74" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="59"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="68"/>
-    </row>
-    <row r="22" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="76" t="s">
+      <c r="C22" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="E22" s="71" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" s="73" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="60"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="67"/>
+    </row>
+    <row r="24" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B22" s="76" t="s">
-        <v>172</v>
-      </c>
-      <c r="C22" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="D22" s="76" t="s">
+      <c r="B24" s="75" t="s">
         <v>173</v>
       </c>
-      <c r="E22" s="72" t="s">
-        <v>150</v>
-      </c>
-      <c r="F22" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G22" s="74" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="61"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="68"/>
-    </row>
-    <row r="24" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="76" t="s">
-        <v>163</v>
-      </c>
-      <c r="B24" s="76" t="s">
+      <c r="C24" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="75" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="D24" s="76" t="s">
+      <c r="E24" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" s="73" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="60"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="67"/>
+    </row>
+    <row r="26" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="75" t="s">
+        <v>177</v>
+      </c>
+      <c r="B26" s="75" t="s">
         <v>175</v>
       </c>
-      <c r="E24" s="72" t="s">
-        <v>153</v>
-      </c>
-      <c r="F24" s="73" t="s">
-        <v>135</v>
-      </c>
-      <c r="G24" s="74" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="61"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="68"/>
-    </row>
-    <row r="26" spans="1:7" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="76" t="s">
-        <v>178</v>
-      </c>
-      <c r="B26" s="76" t="s">
+      <c r="C26" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="75" t="s">
         <v>176</v>
       </c>
-      <c r="C26" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="D26" s="76" t="s">
-        <v>177</v>
-      </c>
-      <c r="E26" s="72" t="s">
+      <c r="E26" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" s="72" t="s">
         <v>156</v>
       </c>
-      <c r="F26" s="73" t="s">
-        <v>157</v>
-      </c>
-      <c r="G26" s="74" t="s">
-        <v>156</v>
+      <c r="G26" s="73" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -4175,7 +4164,7 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4186,7 +4175,7 @@
     <col min="4" max="4" width="28.42578125"/>
     <col min="5" max="5" width="33.42578125"/>
     <col min="6" max="6" width="25.85546875"/>
-    <col min="7" max="7" width="26.7109375" style="65"/>
+    <col min="7" max="7" width="26.7109375" style="64"/>
     <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
@@ -4224,25 +4213,25 @@
         <v>12</v>
       </c>
       <c r="F2" s="32"/>
-      <c r="G2" s="66"/>
+      <c r="G2" s="65"/>
     </row>
     <row r="3" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
-      <c r="G3" s="66"/>
+      <c r="G3" s="65"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E4" s="36"/>
       <c r="F4" s="37"/>
-      <c r="G4" s="67"/>
+      <c r="G4" s="66"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
@@ -4286,18 +4275,18 @@
       <c r="F6" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="63" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="68"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="67"/>
     </row>
     <row r="8" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
@@ -4318,18 +4307,18 @@
       <c r="F8" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="G8" s="64" t="s">
+      <c r="G8" s="63" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="68"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="67"/>
     </row>
     <row r="10" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
@@ -4350,399 +4339,399 @@
       <c r="F10" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="48" t="s">
-        <v>124</v>
+      <c r="G10" s="81" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="49"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="68"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="C12" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="D12" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="E12" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="F12" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="F12" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="G12" s="64" t="s">
-        <v>129</v>
+      <c r="G12" s="63" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="68"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="C14" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="D14" s="45" t="s">
+      <c r="F14" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="E14" s="46" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="G14" s="64" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="68"/>
+      <c r="A15" s="48"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="67"/>
     </row>
     <row r="16" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A16" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="C16" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="D16" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="E16" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="F16" s="51" t="s">
         <v>201</v>
       </c>
-      <c r="F16" s="52" t="s">
+      <c r="G16" s="80" t="s">
         <v>202</v>
       </c>
-      <c r="G16" s="81" t="s">
-        <v>203</v>
-      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="54"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="68"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="67"/>
     </row>
     <row r="18" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="44"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="69"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="68"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="59"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="68"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="67"/>
     </row>
     <row r="20" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="44"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="69"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="68"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="61"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="68"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="67"/>
     </row>
     <row r="22" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="44"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="69"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="68"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="61"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="68"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="67"/>
     </row>
     <row r="24" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="44"/>
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="69"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="68"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="54"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="68"/>
+      <c r="A25" s="53"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="67"/>
     </row>
     <row r="26" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="44"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="69"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="68"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="54"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="68"/>
+      <c r="A27" s="53"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="67"/>
     </row>
     <row r="28" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
-      <c r="D28" s="55"/>
+      <c r="D28" s="54"/>
       <c r="E28" s="46"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="69"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="68"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="68"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="67"/>
     </row>
     <row r="30" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44"/>
       <c r="B30" s="45"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="69"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="68"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="49"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="68"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="67"/>
     </row>
     <row r="32" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="44"/>
       <c r="B32" s="45"/>
       <c r="C32" s="45"/>
-      <c r="D32" s="55"/>
+      <c r="D32" s="54"/>
       <c r="E32" s="46"/>
       <c r="F32" s="47"/>
-      <c r="G32" s="69"/>
+      <c r="G32" s="68"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="49"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="68"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="67"/>
     </row>
     <row r="34" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="44"/>
       <c r="B34" s="45"/>
       <c r="C34" s="45"/>
-      <c r="D34" s="55"/>
+      <c r="D34" s="54"/>
       <c r="E34" s="46"/>
       <c r="F34" s="47"/>
-      <c r="G34" s="69"/>
+      <c r="G34" s="68"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="49"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="68"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="67"/>
     </row>
     <row r="36" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44"/>
       <c r="B36" s="45"/>
       <c r="C36" s="45"/>
-      <c r="D36" s="55"/>
+      <c r="D36" s="54"/>
       <c r="E36" s="46"/>
       <c r="F36" s="47"/>
-      <c r="G36" s="69"/>
+      <c r="G36" s="68"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="49"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="68"/>
+      <c r="A37" s="48"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="67"/>
     </row>
     <row r="38" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="44"/>
       <c r="B38" s="45"/>
       <c r="C38" s="45"/>
-      <c r="D38" s="55"/>
+      <c r="D38" s="54"/>
       <c r="E38" s="46"/>
       <c r="F38" s="47"/>
-      <c r="G38" s="69"/>
+      <c r="G38" s="68"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="49"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="68"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="67"/>
     </row>
     <row r="40" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="44"/>
       <c r="B40" s="45"/>
       <c r="C40" s="45"/>
-      <c r="D40" s="55"/>
+      <c r="D40" s="54"/>
       <c r="E40" s="46"/>
       <c r="F40" s="47"/>
-      <c r="G40" s="69"/>
+      <c r="G40" s="68"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="62"/>
+      <c r="A41" s="61"/>
       <c r="B41" s="28"/>
       <c r="C41" s="28"/>
       <c r="D41" s="28"/>
       <c r="E41" s="28"/>
       <c r="F41" s="28"/>
-      <c r="G41" s="70"/>
+      <c r="G41" s="69"/>
     </row>
     <row r="42" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="44"/>
       <c r="B42" s="45"/>
       <c r="C42" s="45"/>
-      <c r="D42" s="55"/>
+      <c r="D42" s="54"/>
       <c r="E42" s="46"/>
       <c r="F42" s="47"/>
-      <c r="G42" s="69"/>
+      <c r="G42" s="68"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="62"/>
+      <c r="A43" s="61"/>
       <c r="B43" s="28"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
-      <c r="G43" s="70"/>
+      <c r="G43" s="69"/>
     </row>
     <row r="44" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="44"/>
-      <c r="B44" s="55"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="69"/>
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="68"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="62"/>
+      <c r="A45" s="61"/>
       <c r="G45"/>
     </row>
     <row r="46" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="44"/>
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="69"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="68"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="62"/>
+      <c r="A47" s="61"/>
       <c r="G47"/>
     </row>
     <row r="48" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="44"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="69"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="54"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="68"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="62"/>
+      <c r="A49" s="61"/>
       <c r="G49"/>
     </row>
     <row r="50" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="44"/>
-      <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="69"/>
+      <c r="B50" s="54"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="68"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="62"/>
+      <c r="A51" s="61"/>
       <c r="G51"/>
     </row>
     <row r="52" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4752,10 +4741,10 @@
       <c r="D52" s="45"/>
       <c r="E52" s="46"/>
       <c r="F52" s="47"/>
-      <c r="G52" s="69"/>
+      <c r="G52" s="68"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="62"/>
+      <c r="A53" s="61"/>
       <c r="G53"/>
     </row>
     <row r="54" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4765,10 +4754,10 @@
       <c r="D54" s="45"/>
       <c r="E54" s="46"/>
       <c r="F54" s="47"/>
-      <c r="G54" s="69"/>
+      <c r="G54" s="68"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="62"/>
+      <c r="A55" s="61"/>
       <c r="G55"/>
     </row>
     <row r="56" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4778,7 +4767,7 @@
       <c r="D56" s="45"/>
       <c r="E56" s="46"/>
       <c r="F56" s="47"/>
-      <c r="G56" s="69"/>
+      <c r="G56" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4834,7 +4823,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="31"/>
@@ -4848,11 +4837,11 @@
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="87" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
+      <c r="B3" s="86" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
       <c r="E3" s="34"/>
       <c r="F3" s="35"/>
       <c r="G3" s="33"/>
@@ -4886,304 +4875,304 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="77" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="78" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="C6" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="78" t="s">
         <v>193</v>
       </c>
-      <c r="C6" s="79" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="79" t="s">
+      <c r="E6" s="46" t="s">
         <v>194</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>195</v>
       </c>
       <c r="F6" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="75" t="s">
-        <v>196</v>
+      <c r="G6" s="74" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="49"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
     </row>
     <row r="8" spans="1:7" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="77" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" s="78" t="s">
         <v>204</v>
       </c>
-      <c r="B8" s="79" t="s">
+      <c r="C8" s="77" t="s">
         <v>205</v>
       </c>
-      <c r="C8" s="78" t="s">
+      <c r="D8" s="78" t="s">
         <v>206</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="E8" s="46" t="s">
         <v>207</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>208</v>
       </c>
       <c r="F8" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="75" t="s">
-        <v>196</v>
+      <c r="G8" s="74" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="54"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
     </row>
     <row r="10" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="58"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="57"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="59"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
     </row>
     <row r="12" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="78"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="58"/>
+      <c r="A12" s="77"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="57"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="61"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="78"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="58"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="61"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
     </row>
     <row r="16" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="78"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="58"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="57"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="54"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
     </row>
     <row r="18" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="78"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="58"/>
+      <c r="A18" s="77"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="57"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="54"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
     </row>
     <row r="20" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="78"/>
-      <c r="B20" s="79"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="55"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="46"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="53"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
     </row>
     <row r="22" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="78"/>
-      <c r="B22" s="79"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="53"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="52"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
     </row>
     <row r="24" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="78"/>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="55"/>
+      <c r="A24" s="77"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="46"/>
       <c r="F24" s="47"/>
-      <c r="G24" s="53"/>
+      <c r="G24" s="52"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="49"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
     </row>
     <row r="26" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="78"/>
-      <c r="B26" s="79"/>
-      <c r="C26" s="79"/>
-      <c r="D26" s="55"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="78"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="46"/>
       <c r="F26" s="47"/>
-      <c r="G26" s="53"/>
+      <c r="G26" s="52"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
     </row>
     <row r="28" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="78"/>
-      <c r="B28" s="79"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="55"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="54"/>
       <c r="E28" s="46"/>
       <c r="F28" s="47"/>
-      <c r="G28" s="53"/>
+      <c r="G28" s="52"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="78"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="58"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="57"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="49"/>
+      <c r="A31" s="48"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="78"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="58"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="57"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="49"/>
+      <c r="A33" s="48"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="78"/>
-      <c r="B34" s="55"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="56"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="58"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="57"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="49"/>
+      <c r="A35" s="48"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="78"/>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="58"/>
+      <c r="A36" s="77"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="57"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="49"/>
+      <c r="A37" s="48"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="78"/>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="58"/>
+      <c r="A38" s="77"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>